<commit_message>
average test score function
</commit_message>
<xml_diff>
--- a/r2 scores.xlsx
+++ b/r2 scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tenni\Documents\GitHub\Gervigreind Lokaverkefni\GervigreindFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCE8A5D-E3EB-4E48-BC3D-7028F8FBF664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3959921B-15E1-4B48-B271-74739ACFCCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="63240" yWindow="3825" windowWidth="13800" windowHeight="15105" xr2:uid="{A87E3430-8687-47C2-92DD-7B9C2E83BA30}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Best r2 scores Copenhagen</t>
   </si>
@@ -50,18 +50,38 @@
     <t>Linear Regression with LOOCV</t>
   </si>
   <si>
-    <t>Linear Regression (average of 10 train/test splits)</t>
-  </si>
-  <si>
     <t>*LOOCV = leave-one-out cross validation</t>
+  </si>
+  <si>
+    <t>NuSVR (average*)</t>
+  </si>
+  <si>
+    <t>Linear Regression (average*)</t>
+  </si>
+  <si>
+    <t>*average = average score of model with 10 train/test splits</t>
+  </si>
+  <si>
+    <t>Gradient Regression Boost (average*)</t>
+  </si>
+  <si>
+    <t>Gradient Regression Boost with LOOCV (5000 samples)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -89,8 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,46 +426,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC86E81-6AC2-483F-A386-E62E818A41ED}">
-  <dimension ref="B1:D5"/>
+  <dimension ref="B1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="42.59765625" customWidth="1"/>
+    <col min="2" max="2" width="46.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>3</v>
       </c>
+      <c r="C5">
+        <v>0.57399999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>0.56899999999999995</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All test sizes for average score = 0.2
</commit_message>
<xml_diff>
--- a/r2 scores.xlsx
+++ b/r2 scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tenni\Documents\GitHub\Gervigreind Lokaverkefni\GervigreindFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB1AF54-E185-4E64-B9DE-91738703BCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B559BE-A8EE-4FFC-87C9-8181339DC41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63240" yWindow="3825" windowWidth="13800" windowHeight="15105" xr2:uid="{A87E3430-8687-47C2-92DD-7B9C2E83BA30}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A87E3430-8687-47C2-92DD-7B9C2E83BA30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Best r2 scores Copenhagen</t>
   </si>
@@ -47,47 +47,50 @@
     <t>*LOOCV = leave-one-out cross validation</t>
   </si>
   <si>
-    <t>NuSVR (average*)</t>
-  </si>
-  <si>
-    <t>Linear Regression (average*)</t>
-  </si>
-  <si>
-    <t>Gradient boosting regression (average*)</t>
-  </si>
-  <si>
-    <t>Gradient boosting regression with LOOCV (5000 samples)</t>
-  </si>
-  <si>
-    <t>Gradient boosting regression with LOOCV (entire dataset)</t>
-  </si>
-  <si>
-    <t>Random Forest Regressor (average*)</t>
-  </si>
-  <si>
     <t>*average = average score of model with 10 different train/test splits</t>
   </si>
   <si>
-    <t>Random Forest Regressor LOOCV</t>
-  </si>
-  <si>
-    <t>Linear Regression LOOCV</t>
-  </si>
-  <si>
     <t>Neural Network</t>
   </si>
   <si>
     <t>GBR 5000 datapoints</t>
   </si>
   <si>
-    <t>r2 test score</t>
+    <t>Train r2</t>
+  </si>
+  <si>
+    <t>Test r2</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>LOOCV</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>NuSVR</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Gradient Boosting</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
+  <si>
+    <t>Eval method</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +102,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,12 +133,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -151,16 +162,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9732</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>638382</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>618985</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>599935</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -183,7 +194,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5505657" y="762000"/>
+          <a:off x="4953207" y="828675"/>
           <a:ext cx="3847753" cy="3162300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -493,113 +504,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC86E81-6AC2-483F-A386-E62E818A41ED}">
-  <dimension ref="B1:J12"/>
+  <dimension ref="B1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.53125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="D1" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.51549999999999996</v>
+      </c>
+      <c r="E5">
+        <v>0.51470000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0.621</v>
+      </c>
+      <c r="E6">
+        <v>0.5363</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>0.54179999999999995</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>0.53580000000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>0.54249999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>0.60760000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>0.56899999999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>0.53469999999999995</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
+      <c r="C10" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
all models r2 scores calculated
</commit_message>
<xml_diff>
--- a/r2 scores.xlsx
+++ b/r2 scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tenni\Documents\GitHub\Gervigreind Lokaverkefni\GervigreindFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B559BE-A8EE-4FFC-87C9-8181339DC41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FD42AF-420E-4AC6-A8F1-1C4FA07BBD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A87E3430-8687-47C2-92DD-7B9C2E83BA30}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +111,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="5"/>
+      <color rgb="FF7F848E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -141,6 +148,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC86E81-6AC2-483F-A386-E62E818A41ED}">
-  <dimension ref="B1:M10"/>
+  <dimension ref="B1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -551,6 +561,9 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
+      <c r="E4">
+        <v>0.53600000000000003</v>
+      </c>
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
@@ -568,10 +581,10 @@
         <v>10</v>
       </c>
       <c r="D5" s="4">
-        <v>0.51549999999999996</v>
+        <v>0.54179999999999995</v>
       </c>
       <c r="E5">
-        <v>0.51470000000000005</v>
+        <v>0.53749999999999998</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.45">
@@ -582,10 +595,10 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>0.621</v>
+        <v>0.64690000000000003</v>
       </c>
       <c r="E6">
-        <v>0.5363</v>
+        <v>0.55020000000000002</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.45">
@@ -595,6 +608,12 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
+      <c r="D7">
+        <v>0.79610000000000003</v>
+      </c>
+      <c r="E7">
+        <v>0.59689999999999999</v>
+      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
@@ -603,6 +622,12 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
+      <c r="D8">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.54510000000000003</v>
+      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
@@ -611,6 +636,12 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
+      <c r="D9">
+        <v>0.73760000000000003</v>
+      </c>
+      <c r="E9">
+        <v>0.58309999999999995</v>
+      </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
@@ -619,6 +650,15 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
+      <c r="D10">
+        <v>0.59140000000000004</v>
+      </c>
+      <c r="E10">
+        <v>0.56089999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C17" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
scores stockholm, london, paris
</commit_message>
<xml_diff>
--- a/r2 scores.xlsx
+++ b/r2 scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tenni\Documents\GitHub\Gervigreind Lokaverkefni\GervigreindFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4646866-C071-4B9A-AE12-DB9052ACC0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB581C4-D5CC-4920-850C-96608A57E871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A87E3430-8687-47C2-92DD-7B9C2E83BA30}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
   <si>
     <t>Best r2 scores Copenhagen</t>
   </si>
@@ -84,13 +84,22 @@
   </si>
   <si>
     <t>Average score</t>
+  </si>
+  <si>
+    <t>Best r2 scores Stockholm</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Paris</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,13 +120,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="5"/>
-      <color rgb="FF7F848E"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -148,9 +150,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC86E81-6AC2-483F-A386-E62E818A41ED}">
-  <dimension ref="B1:M17"/>
+  <dimension ref="B1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -547,10 +546,10 @@
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -657,12 +656,219 @@
         <v>0.56089999999999995</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C17" s="5"/>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>0.57399999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="E16">
+        <v>0.55589999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>0.7208</v>
+      </c>
+      <c r="E17">
+        <v>0.5857</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>0.94340000000000002</v>
+      </c>
+      <c r="E18">
+        <v>0.60599999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>0.87639999999999996</v>
+      </c>
+      <c r="E19">
+        <v>0.60250000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="E20">
+        <v>0.61750000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>0.63349999999999995</v>
+      </c>
+      <c r="E21">
+        <v>0.59050000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>0.86760000000000004</v>
+      </c>
+      <c r="E26">
+        <v>0.65959999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="E27">
+        <v>0.64549999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>0.85360000000000003</v>
+      </c>
+      <c r="E31">
+        <v>0.7409</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="E32">
+        <v>0.70520000000000005</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>